<commit_message>
add images and change in files
</commit_message>
<xml_diff>
--- a/excelfiles/Product Inventory Template.xlsx
+++ b/excelfiles/Product Inventory Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\personal proj\project1\citymart\excelfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7DE3D0-550A-42E4-9B53-1ED49B2F0922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECBEA1B-612D-44A6-A311-FF56EDB9C209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E91D1D6E-9C6B-49FE-86E8-D0083A4A6406}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="61">
   <si>
     <t>Product Code</t>
   </si>
@@ -68,40 +68,157 @@
     <t>Last Purchase Date</t>
   </si>
   <si>
-    <t>Silver Coin Atta</t>
-  </si>
-  <si>
-    <t>products/silvercoin.jpeg</t>
-  </si>
-  <si>
-    <t>5 Kg</t>
-  </si>
-  <si>
     <t>Flour (Atta)</t>
   </si>
   <si>
-    <t>10 Kg</t>
-  </si>
-  <si>
-    <t>Ahsirwaad Atta</t>
-  </si>
-  <si>
-    <t>products/ashirwaad.webp</t>
-  </si>
-  <si>
-    <t>Organic Atta</t>
-  </si>
-  <si>
-    <t>products/organic.webp</t>
-  </si>
-  <si>
-    <t>Deepak Atta</t>
-  </si>
-  <si>
-    <t>products/deepak.jpg</t>
-  </si>
-  <si>
     <t>MRP</t>
+  </si>
+  <si>
+    <t>Fortune Chakki Atta</t>
+  </si>
+  <si>
+    <t>products/fortune.webp</t>
+  </si>
+  <si>
+    <t>5 kg</t>
+  </si>
+  <si>
+    <t>10 kg</t>
+  </si>
+  <si>
+    <t>Tata Tea Premium</t>
+  </si>
+  <si>
+    <t>500 gm</t>
+  </si>
+  <si>
+    <t>Beverages</t>
+  </si>
+  <si>
+    <t>Brooke Bond Red Label</t>
+  </si>
+  <si>
+    <t>Taj Mahal Tea</t>
+  </si>
+  <si>
+    <t>250gm</t>
+  </si>
+  <si>
+    <t>Nescafé Classic Coffee</t>
+  </si>
+  <si>
+    <t>100 gm</t>
+  </si>
+  <si>
+    <t>Bru Instant Coffee</t>
+  </si>
+  <si>
+    <t>Horlicks</t>
+  </si>
+  <si>
+    <t>Bournvita</t>
+  </si>
+  <si>
+    <t>Complan</t>
+  </si>
+  <si>
+    <t>Boost</t>
+  </si>
+  <si>
+    <t>PediaSure</t>
+  </si>
+  <si>
+    <t>400 gm</t>
+  </si>
+  <si>
+    <t>Real Fruit Juice</t>
+  </si>
+  <si>
+    <t>1L</t>
+  </si>
+  <si>
+    <t>Tropicana Juice</t>
+  </si>
+  <si>
+    <t>Paper Boat Juice</t>
+  </si>
+  <si>
+    <t>250ml</t>
+  </si>
+  <si>
+    <t>Coca-Cola</t>
+  </si>
+  <si>
+    <t>750ml</t>
+  </si>
+  <si>
+    <t>2.25L</t>
+  </si>
+  <si>
+    <t>Pepsi</t>
+  </si>
+  <si>
+    <t>Sprite</t>
+  </si>
+  <si>
+    <t>Thums Up</t>
+  </si>
+  <si>
+    <t>Fanta</t>
+  </si>
+  <si>
+    <t>products/tata_premium.jpg</t>
+  </si>
+  <si>
+    <t>products/nescafé_coffee.jpg</t>
+  </si>
+  <si>
+    <t>products/bru_coffee.jpg</t>
+  </si>
+  <si>
+    <t>products/real_juice.jpg</t>
+  </si>
+  <si>
+    <t>products/coca_cola.jpg</t>
+  </si>
+  <si>
+    <t>products/brooke_bond.jpg</t>
+  </si>
+  <si>
+    <t>products/taj_mahal.jpg</t>
+  </si>
+  <si>
+    <t>products/Horlicks.jpg</t>
+  </si>
+  <si>
+    <t>products/bournvita.jpg</t>
+  </si>
+  <si>
+    <t>products/complan.jpg</t>
+  </si>
+  <si>
+    <t>products/boost.jpg</t>
+  </si>
+  <si>
+    <t>products/pediasure.jpg</t>
+  </si>
+  <si>
+    <t>products/pepsi.jpg</t>
+  </si>
+  <si>
+    <t>products/fanta.jpg</t>
+  </si>
+  <si>
+    <t>products/thums_up.webp</t>
+  </si>
+  <si>
+    <t>products/sprite.webp</t>
+  </si>
+  <si>
+    <t>products/tropicana_juice.jpg</t>
+  </si>
+  <si>
+    <t>products/paper_boat.jpeg</t>
   </si>
 </sst>
 </file>
@@ -512,22 +629,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B69204D3-D303-40FF-B6D7-C87B883172E8}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.77734375" bestFit="1" customWidth="1"/>
@@ -556,7 +673,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>7</v>
@@ -570,287 +687,1113 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1001</v>
+        <v>1009</v>
       </c>
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
       <c r="F2">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G2">
-        <v>240</v>
+        <v>420</v>
       </c>
       <c r="H2">
-        <v>260</v>
+        <v>445</v>
       </c>
       <c r="I2">
-        <v>250</v>
+        <v>434</v>
       </c>
       <c r="J2" s="4">
-        <v>45536</v>
+        <f ca="1">NOW()</f>
+        <v>45546.94045671296</v>
       </c>
       <c r="K2" s="4">
-        <v>45536</v>
+        <f ca="1">NOW()</f>
+        <v>45546.94045671296</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1002</v>
+        <v>1010</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F3">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="G3">
-        <v>410</v>
+        <v>200</v>
       </c>
       <c r="H3">
-        <v>450</v>
+        <v>230</v>
       </c>
       <c r="I3">
-        <v>430</v>
+        <v>210</v>
       </c>
       <c r="J3" s="4">
-        <v>45536</v>
+        <f ca="1">NOW()</f>
+        <v>45546.94045671296</v>
       </c>
       <c r="K3" s="4">
-        <v>45536</v>
+        <f ca="1">NOW()</f>
+        <v>45546.94045671296</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>1003</v>
+        <v>2001</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G4">
+        <v>230</v>
+      </c>
+      <c r="H4">
         <v>250</v>
       </c>
-      <c r="H4">
-        <v>280</v>
-      </c>
       <c r="I4">
-        <v>265</v>
+        <v>240</v>
       </c>
       <c r="J4" s="4">
-        <v>45536</v>
+        <f t="shared" ref="J4:K31" ca="1" si="0">NOW()</f>
+        <v>45546.94045671296</v>
       </c>
       <c r="K4" s="4">
-        <v>45536</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>1004</v>
+        <v>2002</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F5">
         <v>20</v>
       </c>
       <c r="G5">
-        <v>405</v>
+        <v>220</v>
       </c>
       <c r="H5">
-        <v>440</v>
+        <v>240</v>
       </c>
       <c r="I5">
-        <v>425</v>
+        <v>230</v>
       </c>
       <c r="J5" s="4">
-        <v>45536</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
       </c>
       <c r="K5" s="4">
-        <v>45536</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>1005</v>
+        <v>2003</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F6">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G6">
-        <v>230</v>
+        <v>170</v>
       </c>
       <c r="H6">
-        <v>275</v>
+        <v>190</v>
       </c>
       <c r="I6">
-        <v>255</v>
+        <v>180</v>
       </c>
       <c r="J6" s="4">
-        <v>45536</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
       </c>
       <c r="K6" s="4">
-        <v>45536</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>1006</v>
+        <v>2004</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F7">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="G7">
-        <v>400</v>
+        <v>175</v>
       </c>
       <c r="H7">
-        <v>435</v>
+        <v>210</v>
       </c>
       <c r="I7">
-        <v>420</v>
+        <v>195</v>
       </c>
       <c r="J7" s="4">
-        <v>45536</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
       </c>
       <c r="K7" s="4">
-        <v>45536</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>1007</v>
+        <v>2005</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F8">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="G8">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="H8">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="I8">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="J8" s="4">
-        <v>45536</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
       </c>
       <c r="K8" s="4">
-        <v>45536</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>1008</v>
+        <v>2006</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9">
         <v>20</v>
       </c>
-      <c r="D9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9">
-        <v>7</v>
-      </c>
       <c r="G9">
-        <v>399</v>
+        <v>250</v>
       </c>
       <c r="H9">
-        <v>445</v>
+        <v>280</v>
       </c>
       <c r="I9">
-        <v>420</v>
+        <v>260</v>
       </c>
       <c r="J9" s="4">
-        <v>45536</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
       </c>
       <c r="K9" s="4">
-        <v>45536</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
+      <c r="A10">
+        <v>2007</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10">
+        <v>25</v>
+      </c>
+      <c r="G10">
+        <v>230</v>
+      </c>
+      <c r="H10">
+        <v>250</v>
+      </c>
+      <c r="I10">
+        <v>240</v>
+      </c>
+      <c r="J10" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+      <c r="K10" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2008</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11">
+        <v>25</v>
+      </c>
+      <c r="G11">
+        <v>290</v>
+      </c>
+      <c r="H11">
+        <v>320</v>
+      </c>
+      <c r="I11">
+        <v>299</v>
+      </c>
+      <c r="J11" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+      <c r="K11" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2009</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12">
+        <v>25</v>
+      </c>
+      <c r="G12">
+        <v>260</v>
+      </c>
+      <c r="H12">
+        <v>290</v>
+      </c>
+      <c r="I12">
+        <v>280</v>
+      </c>
+      <c r="J12" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+      <c r="K12" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>2010</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13">
+        <v>25</v>
+      </c>
+      <c r="G13">
+        <v>500</v>
+      </c>
+      <c r="H13">
+        <v>550</v>
+      </c>
+      <c r="I13">
+        <v>525</v>
+      </c>
+      <c r="J13" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+      <c r="K13" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2011</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14">
+        <v>30</v>
+      </c>
+      <c r="G14">
+        <v>100</v>
+      </c>
+      <c r="H14">
+        <v>120</v>
+      </c>
+      <c r="I14">
+        <v>110</v>
+      </c>
+      <c r="J14" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+      <c r="K14" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>2012</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15">
+        <v>30</v>
+      </c>
+      <c r="G15">
+        <v>110</v>
+      </c>
+      <c r="H15">
+        <v>130</v>
+      </c>
+      <c r="I15">
+        <v>99</v>
+      </c>
+      <c r="J15" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+      <c r="K15" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>2013</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16">
+        <v>50</v>
+      </c>
+      <c r="G16">
+        <v>30</v>
+      </c>
+      <c r="H16">
+        <v>40</v>
+      </c>
+      <c r="I16">
+        <v>35</v>
+      </c>
+      <c r="J16" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+      <c r="K16" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>2014</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17">
+        <v>50</v>
+      </c>
+      <c r="G17">
+        <v>40</v>
+      </c>
+      <c r="H17">
+        <v>45</v>
+      </c>
+      <c r="I17">
+        <v>42</v>
+      </c>
+      <c r="J17" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+      <c r="K17" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2015</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18">
+        <v>30</v>
+      </c>
+      <c r="G18">
+        <v>60</v>
+      </c>
+      <c r="H18">
+        <v>70</v>
+      </c>
+      <c r="I18">
+        <v>65</v>
+      </c>
+      <c r="J18" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+      <c r="K18" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>2016</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19">
+        <v>20</v>
+      </c>
+      <c r="G19">
+        <v>85</v>
+      </c>
+      <c r="H19">
+        <v>110</v>
+      </c>
+      <c r="I19">
+        <v>99</v>
+      </c>
+      <c r="J19" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+      <c r="K19" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2017</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20">
+        <v>50</v>
+      </c>
+      <c r="G20">
+        <v>40</v>
+      </c>
+      <c r="H20">
+        <v>45</v>
+      </c>
+      <c r="I20">
+        <v>42</v>
+      </c>
+      <c r="J20" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+      <c r="K20" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2018</v>
+      </c>
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21">
+        <v>30</v>
+      </c>
+      <c r="G21">
+        <v>60</v>
+      </c>
+      <c r="H21">
+        <v>70</v>
+      </c>
+      <c r="I21">
+        <v>65</v>
+      </c>
+      <c r="J21" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+      <c r="K21" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>2019</v>
+      </c>
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22">
+        <v>20</v>
+      </c>
+      <c r="G22">
+        <v>85</v>
+      </c>
+      <c r="H22">
+        <v>110</v>
+      </c>
+      <c r="I22">
+        <v>99</v>
+      </c>
+      <c r="J22" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+      <c r="K22" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2020</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23">
+        <v>60</v>
+      </c>
+      <c r="G23">
+        <v>40</v>
+      </c>
+      <c r="H23">
+        <v>45</v>
+      </c>
+      <c r="I23">
+        <v>42</v>
+      </c>
+      <c r="J23" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+      <c r="K23" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>2021</v>
+      </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24">
+        <v>45</v>
+      </c>
+      <c r="G24">
+        <v>60</v>
+      </c>
+      <c r="H24">
+        <v>70</v>
+      </c>
+      <c r="I24">
+        <v>65</v>
+      </c>
+      <c r="J24" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+      <c r="K24" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>2022</v>
+      </c>
+      <c r="B25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25">
+        <v>40</v>
+      </c>
+      <c r="G25">
+        <v>85</v>
+      </c>
+      <c r="H25">
+        <v>110</v>
+      </c>
+      <c r="I25">
+        <v>99</v>
+      </c>
+      <c r="J25" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+      <c r="K25" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>2023</v>
+      </c>
+      <c r="B26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26">
+        <v>30</v>
+      </c>
+      <c r="G26">
+        <v>40</v>
+      </c>
+      <c r="H26">
+        <v>45</v>
+      </c>
+      <c r="I26">
+        <v>42</v>
+      </c>
+      <c r="J26" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+      <c r="K26" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>2024</v>
+      </c>
+      <c r="B27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27">
+        <v>20</v>
+      </c>
+      <c r="G27">
+        <v>60</v>
+      </c>
+      <c r="H27">
+        <v>70</v>
+      </c>
+      <c r="I27">
+        <v>65</v>
+      </c>
+      <c r="J27" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+      <c r="K27" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>2025</v>
+      </c>
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28">
+        <v>25</v>
+      </c>
+      <c r="G28">
+        <v>85</v>
+      </c>
+      <c r="H28">
+        <v>110</v>
+      </c>
+      <c r="I28">
+        <v>99</v>
+      </c>
+      <c r="J28" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+      <c r="K28" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>2026</v>
+      </c>
+      <c r="B29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29">
+        <v>30</v>
+      </c>
+      <c r="G29">
+        <v>40</v>
+      </c>
+      <c r="H29">
+        <v>45</v>
+      </c>
+      <c r="I29">
+        <v>42</v>
+      </c>
+      <c r="J29" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+      <c r="K29" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>2027</v>
+      </c>
+      <c r="B30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30">
+        <v>25</v>
+      </c>
+      <c r="G30">
+        <v>60</v>
+      </c>
+      <c r="H30">
+        <v>70</v>
+      </c>
+      <c r="I30">
+        <v>65</v>
+      </c>
+      <c r="J30" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+      <c r="K30" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>2028</v>
+      </c>
+      <c r="B31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31">
+        <v>10</v>
+      </c>
+      <c r="G31">
+        <v>85</v>
+      </c>
+      <c r="H31">
+        <v>110</v>
+      </c>
+      <c r="I31">
+        <v>99</v>
+      </c>
+      <c r="J31" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
+      <c r="K31" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45546.94045671296</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>